<commit_message>
precompile assets, rename drop location column, fixed bugs found by Anne
</commit_message>
<xml_diff>
--- a/import_files/full_bios.xlsx
+++ b/import_files/full_bios.xlsx
@@ -19,7 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="171">
+  <si>
+    <t xml:space="preserve">Oakland  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oakland</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Xochi is working on getting her associate's degree part time, and spends every free moment she can with Samuel and Mateo. She loves to cook and listen to opera.</t>
   </si>
@@ -137,9 +145,6 @@
     <t>Jesus is a great dad, and loves playing hide and seek with Samuel. He also likes woodworking and video games.</t>
   </si>
   <si>
-    <t>DR5K</t>
-  </si>
-  <si>
     <t>Xochitl</t>
   </si>
   <si>
@@ -162,10 +167,6 @@
   </si>
   <si>
     <t>Joseph is a happy baby and loves to smile.</t>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ed is a great dad who loves computers, and has been keeping his old 2000 laptop working for a long time.</t>
@@ -533,6 +534,13 @@
   </si>
   <si>
     <t>Frances</t>
+  </si>
+  <si>
+    <t>drop_location_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5K</t>
   </si>
 </sst>
 </file>
@@ -915,8 +923,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
@@ -953,7 +961,7 @@
         <v>91</v>
       </c>
       <c r="J1" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
       <c r="K1" t="s">
         <v>108</v>
@@ -1003,7 +1011,7 @@
         <v>118</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>119</v>
@@ -1057,7 +1065,7 @@
         <v>118</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>130</v>
@@ -1389,7 +1397,7 @@
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I10" t="s">
         <v>160</v>
@@ -1407,15 +1415,15 @@
         <v>138</v>
       </c>
       <c r="N10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1424,19 +1432,19 @@
         <v>126</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
         <v>128</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I11" t="s">
         <v>160</v>
@@ -1445,10 +1453,10 @@
         <v>95</v>
       </c>
       <c r="K11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M11" t="s">
         <v>92</v>
@@ -1457,7 +1465,7 @@
         <v>93</v>
       </c>
       <c r="O11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1679,7 +1687,7 @@
         <v>67</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>68</v>
@@ -1745,10 +1753,10 @@
         <v>138</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -1864,16 +1872,16 @@
         <v>126</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
         <v>128</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H20" t="s">
         <v>81</v>
@@ -1885,10 +1893,10 @@
         <v>96</v>
       </c>
       <c r="K20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M20" t="s">
         <v>92</v>
@@ -1897,7 +1905,7 @@
         <v>93</v>
       </c>
       <c r="O20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -1947,7 +1955,7 @@
         <v>86</v>
       </c>
       <c r="P21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -2023,7 +2031,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>89</v>
@@ -2052,7 +2060,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
@@ -2073,7 +2081,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>89</v>
@@ -2082,7 +2090,7 @@
         <v>96</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>167</v>
@@ -2127,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>89</v>
@@ -2145,10 +2153,10 @@
         <v>138</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -2158,7 +2166,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -2167,19 +2175,19 @@
         <v>115</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>89</v>
@@ -2188,10 +2196,10 @@
         <v>96</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>92</v>
@@ -2200,7 +2208,7 @@
         <v>93</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
@@ -2210,7 +2218,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1">
         <v>28</v>
@@ -2222,7 +2230,7 @@
         <v>45</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>128</v>
@@ -2231,10 +2239,10 @@
         <v>10</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>106</v>
@@ -2249,10 +2257,10 @@
         <v>60</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -2262,7 +2270,7 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1">
         <v>25</v>
@@ -2283,25 +2291,25 @@
         <v>4</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>106</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>78</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>79</v>
@@ -2316,7 +2324,7 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B29" s="1">
         <v>5</v>
@@ -2337,10 +2345,10 @@
         <v>5</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>106</v>
@@ -2368,7 +2376,7 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B30">
         <v>28</v>
@@ -2389,10 +2397,10 @@
         <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>106</v>
@@ -2412,7 +2420,7 @@
     </row>
     <row r="31" spans="1:20">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>27</v>
@@ -2433,10 +2441,10 @@
         <v>11</v>
       </c>
       <c r="H31" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" t="s">
         <v>28</v>
-      </c>
-      <c r="I31" t="s">
-        <v>26</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>106</v>
@@ -2451,15 +2459,15 @@
         <v>60</v>
       </c>
       <c r="N31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O31" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:20">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>35</v>
@@ -2480,10 +2488,10 @@
         <v>12</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>106</v>
@@ -2507,7 +2515,7 @@
     </row>
     <row r="33" spans="1:20">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1">
         <v>25</v>
@@ -2528,10 +2536,10 @@
         <v>6</v>
       </c>
       <c r="H33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>106</v>
@@ -2555,7 +2563,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1">
         <v>10</v>
@@ -2576,10 +2584,10 @@
         <v>5</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>106</v>
@@ -2625,7 +2633,7 @@
         <v>64</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>106</v>
@@ -2649,7 +2657,7 @@
     </row>
     <row r="36" spans="1:20">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B36" s="1">
         <v>28</v>
@@ -2661,7 +2669,7 @@
         <v>45</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>128</v>
@@ -2670,10 +2678,10 @@
         <v>10</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>38</v>
+        <v>170</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>106</v>
@@ -2688,10 +2696,10 @@
         <v>60</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -2701,7 +2709,7 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1">
         <v>25</v>
@@ -2722,25 +2730,25 @@
         <v>4</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>38</v>
+        <v>170</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>106</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>78</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>79</v>
@@ -2755,7 +2763,7 @@
     </row>
     <row r="38" spans="1:20">
       <c r="A38" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B38" s="1">
         <v>5</v>
@@ -2776,13 +2784,13 @@
         <v>5</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>38</v>
+        <v>170</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
added strip to family code
</commit_message>
<xml_diff>
--- a/import_files/full_bios.xlsx
+++ b/import_files/full_bios.xlsx
@@ -19,7 +19,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="176">
+  <si>
+    <t>Katrina is a hard-working mom, who is always teaching her kids to be kind people. She loves anything orange!</t>
+  </si>
+  <si>
+    <t>Sabrina</t>
+  </si>
+  <si>
+    <t>Sabrina loves trucks, monkeys, and her siblings. When she's not running around outside, she loves to sing.</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>DR5K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DR5A    </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lloyd</t>
+  </si>
+  <si>
+    <t>Lloyd is a little baby with a big personality. Ed loves to dress him up in flowery onesies.</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>TJ loves baseball, basketball, and animals. His favorite color is orange.</t>
+  </si>
+  <si>
+    <t>rap CDs</t>
+  </si>
+  <si>
+    <t>t shirts</t>
+  </si>
+  <si>
+    <t>belts</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
   <si>
     <t xml:space="preserve">Oakland  </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,16 +186,37 @@
     <t>Katrina</t>
   </si>
   <si>
-    <t>Katrina is a hard-working mom, who is always teaching her kids to be kind people. She loves anything orange!</t>
-  </si>
-  <si>
-    <t>Sabrina</t>
-  </si>
-  <si>
-    <t>Sabrina loves trucks, monkeys, and her siblings. When she's not running around outside, she loves to sing.</t>
-  </si>
-  <si>
-    <t>Jesus</t>
+    <t>Lili works during the daytime while Alberto takes care of Wilfredo, and her favorite part of the day is when they are all at home for an hour. She loves tigers.</t>
+  </si>
+  <si>
+    <t>fixed wheel bicycle</t>
+  </si>
+  <si>
+    <t>ray-ban shades</t>
+  </si>
+  <si>
+    <t>jeans</t>
+  </si>
+  <si>
+    <t>hoodie</t>
+  </si>
+  <si>
+    <t>Wilfredo</t>
+  </si>
+  <si>
+    <t>Will is a happy kid who loves running, jumping, and playing! He also loves octopuses and reading comics.</t>
+  </si>
+  <si>
+    <t>football</t>
+  </si>
+  <si>
+    <t>baseball glove</t>
+  </si>
+  <si>
+    <t>basketball</t>
+  </si>
+  <si>
+    <t>Katy</t>
   </si>
   <si>
     <t>Jesus is a great dad, and loves playing hide and seek with Samuel. He also likes woodworking and video games.</t>
@@ -265,28 +342,41 @@
     <t>robe</t>
   </si>
   <si>
-    <t>Lloyd</t>
-  </si>
-  <si>
-    <t>Lloyd is a little baby with a big personality. Ed loves to dress him up in flowery onesies.</t>
-  </si>
-  <si>
-    <t>TJ</t>
-  </si>
-  <si>
-    <t>TJ loves baseball, basketball, and animals. His favorite color is orange.</t>
-  </si>
-  <si>
-    <t>rap CDs</t>
-  </si>
-  <si>
-    <t>t shirts</t>
-  </si>
-  <si>
-    <t>belts</t>
-  </si>
-  <si>
-    <t>Virginia</t>
+    <t>Katy is supporting her kids while working full-time at a local mall. She loves pop cultural analysis and reading feminist blogs.</t>
+  </si>
+  <si>
+    <t>DR5C</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Chelsea's an active little girl who loves playing baseball and running around.</t>
+  </si>
+  <si>
+    <t>hamster</t>
+  </si>
+  <si>
+    <t>kitten</t>
+  </si>
+  <si>
+    <t>puppy</t>
+  </si>
+  <si>
+    <t>fish tank</t>
+  </si>
+  <si>
+    <t>sweater</t>
+  </si>
+  <si>
+    <t>Frances</t>
+  </si>
+  <si>
+    <t>drop_location_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5K</t>
   </si>
   <si>
     <t>Virginia recently started taking care of her sister's son, Kenny, in addition to her four little ones. She lives alone but has cousins in the area that can help. She loves non-fiction books and gum.</t>
@@ -471,76 +561,6 @@
   </si>
   <si>
     <t>Lili</t>
-  </si>
-  <si>
-    <t>Lili works during the daytime while Alberto takes care of Wilfredo, and her favorite part of the day is when they are all at home for an hour. She loves tigers.</t>
-  </si>
-  <si>
-    <t>fixed wheel bicycle</t>
-  </si>
-  <si>
-    <t>ray-ban shades</t>
-  </si>
-  <si>
-    <t>jeans</t>
-  </si>
-  <si>
-    <t>hoodie</t>
-  </si>
-  <si>
-    <t>Wilfredo</t>
-  </si>
-  <si>
-    <t>Will is a happy kid who loves running, jumping, and playing! He also loves octopuses and reading comics.</t>
-  </si>
-  <si>
-    <t>football</t>
-  </si>
-  <si>
-    <t>baseball glove</t>
-  </si>
-  <si>
-    <t>basketball</t>
-  </si>
-  <si>
-    <t>Katy</t>
-  </si>
-  <si>
-    <t>Katy is supporting her kids while working full-time at a local mall. She loves pop cultural analysis and reading feminist blogs.</t>
-  </si>
-  <si>
-    <t>DR5C</t>
-  </si>
-  <si>
-    <t>Chelsea</t>
-  </si>
-  <si>
-    <t>Chelsea's an active little girl who loves playing baseball and running around.</t>
-  </si>
-  <si>
-    <t>hamster</t>
-  </si>
-  <si>
-    <t>kitten</t>
-  </si>
-  <si>
-    <t>puppy</t>
-  </si>
-  <si>
-    <t>fish tank</t>
-  </si>
-  <si>
-    <t>sweater</t>
-  </si>
-  <si>
-    <t>Frances</t>
-  </si>
-  <si>
-    <t>drop_location_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DR5K</t>
   </si>
 </sst>
 </file>
@@ -923,8 +943,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
@@ -934,69 +954,69 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="F1" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="G1" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="H1" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="I1" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="J1" t="s">
-        <v>169</v>
+        <v>114</v>
       </c>
       <c r="K1" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="L1" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="M1" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="N1" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="O1" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="P1" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1">
         <v>10</v>
@@ -1005,31 +1025,31 @@
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>118</v>
+        <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -1038,46 +1058,46 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>125</v>
+        <v>153</v>
       </c>
       <c r="B3" s="1">
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D3" s="1">
         <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G3" s="1">
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1088,13 +1108,13 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1109,28 +1129,28 @@
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>118</v>
+        <v>6</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -1140,43 +1160,43 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1">
         <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D5" s="1">
         <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G5" s="1">
         <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>143</v>
+        <v>5</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1188,19 +1208,19 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="1" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B6" s="1">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D6" s="1">
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="F6" s="1">
         <v>8</v>
@@ -1209,25 +1229,25 @@
         <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>148</v>
+        <v>52</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>143</v>
+        <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>150</v>
+        <v>54</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>152</v>
+        <v>56</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1238,13 +1258,13 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
-        <v>153</v>
+        <v>57</v>
       </c>
       <c r="B7" s="1">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
@@ -1253,31 +1273,31 @@
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G7" s="1">
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>154</v>
+        <v>58</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>156</v>
+        <v>60</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>157</v>
+        <v>61</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -1288,19 +1308,19 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
       <c r="B8">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -1309,36 +1329,36 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
       <c r="I8" t="s">
-        <v>160</v>
+        <v>7</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K8" t="s">
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="L8" t="s">
-        <v>150</v>
+        <v>54</v>
       </c>
       <c r="M8" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="N8" t="s">
-        <v>152</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>106</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1353,39 +1373,39 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>162</v>
+        <v>107</v>
       </c>
       <c r="I9" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K9" t="s">
-        <v>163</v>
+        <v>108</v>
       </c>
       <c r="L9" t="s">
-        <v>164</v>
+        <v>109</v>
       </c>
       <c r="M9" t="s">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="N9" t="s">
-        <v>166</v>
+        <v>111</v>
       </c>
       <c r="O9" t="s">
-        <v>167</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>113</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -1397,140 +1417,140 @@
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K10" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="L10" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="M10" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="N10" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="O10" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s">
-        <v>160</v>
+        <v>105</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K11" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="M11" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="N11" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="O11" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B12" s="1">
         <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D12" s="1">
         <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G12" s="1">
         <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B13" s="1">
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D13" s="1">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="F13" s="1">
         <v>8</v>
@@ -1539,40 +1559,40 @@
         <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B14" s="1">
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
@@ -1587,38 +1607,38 @@
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D15" s="1">
         <v>2</v>
@@ -1633,46 +1653,46 @@
         <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B16" s="1">
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D16" s="1">
         <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="F16" s="1">
         <v>8</v>
@@ -1681,31 +1701,31 @@
         <v>6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -1714,13 +1734,13 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1735,28 +1755,28 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="I17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -1766,66 +1786,66 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B18">
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D18">
         <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="F18" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G18">
         <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="I18" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="K18" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="L18" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="M18" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="N18" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="O18" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B19">
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D19">
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -1834,145 +1854,145 @@
         <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="K19" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="L19" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="M19" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="N19" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="O19" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="P19" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="K20" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="L20" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="M20" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="N20" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="O20" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="B21">
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D21">
         <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="F21" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G21">
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="K21" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="L21" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="M21" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="N21" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="O21" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="P21" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1">
         <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D22" s="1">
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="F22" s="1">
         <v>10</v>
@@ -1981,25 +2001,25 @@
         <v>7</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -2010,13 +2030,13 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="B23" s="1">
         <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D23" s="1">
         <v>5</v>
@@ -2025,31 +2045,31 @@
         <v>5</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G23" s="1">
         <v>1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -2060,13 +2080,13 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
@@ -2075,37 +2095,37 @@
         <v>4</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>167</v>
+        <v>112</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -2114,13 +2134,13 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -2135,28 +2155,28 @@
         <v>1</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -2166,49 +2186,49 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
@@ -2218,49 +2238,49 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B27" s="1">
         <v>28</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D27" s="1">
         <v>45</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G27" s="1">
         <v>10</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -2270,19 +2290,19 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1">
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D28" s="1">
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="F28" s="1">
         <v>10</v>
@@ -2291,31 +2311,31 @@
         <v>4</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -2324,13 +2344,13 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1">
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D29" s="1">
         <v>5</v>
@@ -2339,34 +2359,34 @@
         <v>5</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G29" s="1">
         <v>5</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
@@ -2376,158 +2396,158 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B30">
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D30">
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="F30" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G30">
         <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="I30" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K30" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="L30" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="M30" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="N30" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:20">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B31">
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D31">
         <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="F31" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G31">
         <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="I31" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K31" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="L31" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="M31" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="N31" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="O31" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:20">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B32" s="1">
         <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D32" s="1">
         <v>36</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G32" s="1">
         <v>12</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="P32" s="1"/>
     </row>
     <row r="33" spans="1:20">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1">
         <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D33" s="1">
         <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="F33" s="1">
         <v>8</v>
@@ -2536,40 +2556,40 @@
         <v>6</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="P33" s="1"/>
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="B34" s="1">
         <v>10</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D34" s="1">
         <v>2</v>
@@ -2584,38 +2604,38 @@
         <v>5</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
     <row r="35" spans="1:20">
       <c r="A35" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B35" s="1">
         <v>2</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D35" s="1">
         <v>2</v>
@@ -2630,76 +2650,76 @@
         <v>2</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="P35" s="1"/>
     </row>
     <row r="36" spans="1:20">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B36" s="1">
         <v>28</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D36" s="1">
         <v>45</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G36" s="1">
         <v>10</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>170</v>
+        <v>115</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -2709,19 +2729,19 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B37" s="1">
         <v>25</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="D37" s="1">
         <v>10</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="F37" s="1">
         <v>10</v>
@@ -2730,31 +2750,31 @@
         <v>4</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>170</v>
+        <v>115</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>151</v>
+        <v>55</v>
       </c>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -2763,13 +2783,13 @@
     </row>
     <row r="38" spans="1:20">
       <c r="A38" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B38" s="1">
         <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D38" s="1">
         <v>5</v>
@@ -2778,34 +2798,34 @@
         <v>5</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G38" s="1">
         <v>5</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
@@ -3254,6 +3274,7 @@
       <c r="T58" s="1"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
added downcase to before save family code
</commit_message>
<xml_diff>
--- a/import_files/full_bios.xlsx
+++ b/import_files/full_bios.xlsx
@@ -19,7 +19,404 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="175">
+  <si>
+    <t>Alberto loves soap operas and taking care of Wilfredo. He works the night shift at a factory, and takes care of his little girl in the day time.</t>
+  </si>
+  <si>
+    <t>DR5B</t>
+  </si>
+  <si>
+    <t>microwave</t>
+  </si>
+  <si>
+    <t>cd player</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>Lili</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DR5A    </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waffle iron</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Maria is a strong little girl who loves ponies, the color red, and playing the ukelele.</t>
+  </si>
+  <si>
+    <t>DR5F</t>
+  </si>
+  <si>
+    <t>Florence</t>
+  </si>
+  <si>
+    <t>Florence works at the hospital, and has been taking college classes to become a nurse. She loves running and playing with her baby.</t>
+  </si>
+  <si>
+    <t>dresses</t>
+  </si>
+  <si>
+    <t>socks</t>
+  </si>
+  <si>
+    <t>bed sheets</t>
+  </si>
+  <si>
+    <t>robe</t>
+  </si>
+  <si>
+    <t>Katy is supporting her kids while working full-time at a local mall. She loves pop cultural analysis and reading feminist blogs.</t>
+  </si>
+  <si>
+    <t>DR5C</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Chelsea's an active little girl who loves playing baseball and running around.</t>
+  </si>
+  <si>
+    <t>hamster</t>
+  </si>
+  <si>
+    <t>kitten</t>
+  </si>
+  <si>
+    <t>puppy</t>
+  </si>
+  <si>
+    <t>fish tank</t>
+  </si>
+  <si>
+    <t>sweater</t>
+  </si>
+  <si>
+    <t>Frances</t>
+  </si>
+  <si>
+    <t>drop_location_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5K</t>
+  </si>
+  <si>
+    <t>Virginia recently started taking care of her sister's son, Kenny, in addition to her four little ones. She lives alone but has cousins in the area that can help. She loves non-fiction books and gum.</t>
+  </si>
+  <si>
+    <t>DR5G</t>
+  </si>
+  <si>
+    <t>Kenny</t>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blankets</t>
+  </si>
+  <si>
+    <t>educational videos</t>
+  </si>
+  <si>
+    <t>Ed</t>
+  </si>
+  <si>
+    <t>Oakland</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Richmond</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shades</t>
+  </si>
+  <si>
+    <t>swim trunks</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>size_pants</t>
+  </si>
+  <si>
+    <t>size_shirt</t>
+  </si>
+  <si>
+    <t>size_dress</t>
+  </si>
+  <si>
+    <t>size_shoes</t>
+  </si>
+  <si>
+    <t>Antioch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bio</t>
+  </si>
+  <si>
+    <t>need1</t>
+  </si>
+  <si>
+    <t>need2</t>
+  </si>
+  <si>
+    <t>need3</t>
+  </si>
+  <si>
+    <t>need4</t>
+  </si>
+  <si>
+    <t>need5</t>
+  </si>
+  <si>
+    <t>need6</t>
+  </si>
+  <si>
+    <t>Fran</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>Lovely stay-at-home mom attending community college classes and trying to earn her associate's degree. She loves romance novels.</t>
+  </si>
+  <si>
+    <t>vacuum cleaner</t>
+  </si>
+  <si>
+    <t>dishes</t>
+  </si>
+  <si>
+    <t>pots/pans</t>
+  </si>
+  <si>
+    <t>dress</t>
+  </si>
+  <si>
+    <t>hat</t>
+  </si>
+  <si>
+    <t>couch</t>
+  </si>
+  <si>
+    <t>Phil Jr.</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Phil Jr is a lovely, hard-working kid who loves to run around outside and play with his younger sisters.</t>
+  </si>
+  <si>
+    <t>toys</t>
+  </si>
+  <si>
+    <t>art supplies</t>
+  </si>
+  <si>
+    <t>guitar</t>
+  </si>
+  <si>
+    <t>drums</t>
+  </si>
+  <si>
+    <t>Arianna</t>
+  </si>
+  <si>
+    <t>Arianna is a spunky little 6 year old who is obsessed with animals and is learning to read very quickly!</t>
+  </si>
+  <si>
+    <t>legos</t>
+  </si>
+  <si>
+    <t>books</t>
+  </si>
+  <si>
+    <t>shirts</t>
+  </si>
+  <si>
+    <t>shoes</t>
+  </si>
+  <si>
+    <t>Alberto</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>Tyler works part-time due to a physical limitation, and isn't able to earn a full salary. He's currently supporting Tyler and himself, and loves the color green and the outdoors.</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Fred is a great dad who loves computers, and has been keeping his old 2000 laptop working for a long time.</t>
+  </si>
+  <si>
+    <t>DR5J</t>
+  </si>
+  <si>
+    <t>Katrina</t>
+  </si>
+  <si>
+    <t>Lili works during the daytime while Alberto takes care of Wilfredo, and her favorite part of the day is when they are all at home for an hour. She loves tigers.</t>
+  </si>
+  <si>
+    <t>fixed wheel bicycle</t>
+  </si>
+  <si>
+    <t>ray-ban shades</t>
+  </si>
+  <si>
+    <t>jeans</t>
+  </si>
+  <si>
+    <t>hoodie</t>
+  </si>
+  <si>
+    <t>Wilfredo</t>
+  </si>
+  <si>
+    <t>Will is a happy kid who loves running, jumping, and playing! He also loves octopuses and reading comics.</t>
+  </si>
+  <si>
+    <t>football</t>
+  </si>
+  <si>
+    <t>baseball glove</t>
+  </si>
+  <si>
+    <t>basketball</t>
+  </si>
+  <si>
+    <t>Katy</t>
+  </si>
+  <si>
+    <t>Jesus is a great dad, and loves playing hide and seek with Samuel. He also likes woodworking and video games.</t>
+  </si>
+  <si>
+    <t>Xochitl</t>
+  </si>
+  <si>
+    <t>Frances is a cute toddler with a big smile. She likes dolls and the color red.</t>
+  </si>
+  <si>
+    <t>teddy bear</t>
+  </si>
+  <si>
+    <t>hats</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Alejandro is an active little boy, who loves drawing and telling his parents stories. His current favorite color is brown.</t>
+  </si>
+  <si>
+    <t>infant</t>
+  </si>
+  <si>
+    <t>Joseph is a happy baby and loves to smile.</t>
+  </si>
+  <si>
+    <t>Ed is a great dad who loves computers, and has been keeping his old 2000 laptop working for a long time.</t>
+  </si>
+  <si>
+    <t>DR5D</t>
+  </si>
+  <si>
+    <t>yo-yo</t>
+  </si>
+  <si>
+    <t>backpack</t>
+  </si>
+  <si>
+    <t>coffee mugs</t>
+  </si>
+  <si>
+    <t>bbq</t>
+  </si>
+  <si>
+    <t>Ginny</t>
+  </si>
+  <si>
+    <t>Ginny is a hard-working mom, who is always teaching her kids to be kind people. She loves anything orange!</t>
+  </si>
+  <si>
+    <t>pet monkey</t>
+  </si>
+  <si>
+    <t>watch</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Kelly loves trucks, monkeys, and her siblings. When she's not running around outside, she loves to sing.</t>
+  </si>
+  <si>
+    <t>pants</t>
+  </si>
+  <si>
+    <t>shirt</t>
+  </si>
+  <si>
+    <t>stuffed animals</t>
+  </si>
+  <si>
+    <t>Isabella</t>
+  </si>
+  <si>
+    <t>Isabella is a smart cookie who loves finger painting, dogs, and Teletubbies.</t>
+  </si>
+  <si>
+    <t>Renata</t>
+  </si>
+  <si>
+    <t>Renatta is working hard to provide for her toddler, Maria, without much family support. When she's not at work she quilts and listens to Taylor Swift.</t>
+  </si>
+  <si>
+    <t>DR5E</t>
+  </si>
+  <si>
+    <t>iron</t>
+  </si>
+  <si>
+    <t>dining table</t>
+  </si>
   <si>
     <t>Katrina is a hard-working mom, who is always teaching her kids to be kind people. She loves anything orange!</t>
   </si>
@@ -41,18 +438,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DR5A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DR5C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">DR5A    </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Lloyd</t>
   </si>
   <si>
@@ -169,398 +558,6 @@
   </si>
   <si>
     <t>Tyler</t>
-  </si>
-  <si>
-    <t>Tyler works part-time due to a physical limitation, and isn't able to earn a full salary. He's currently supporting Tyler and himself, and loves the color green and the outdoors.</t>
-  </si>
-  <si>
-    <t>Fred</t>
-  </si>
-  <si>
-    <t>Fred is a great dad who loves computers, and has been keeping his old 2000 laptop working for a long time.</t>
-  </si>
-  <si>
-    <t>DR5J</t>
-  </si>
-  <si>
-    <t>Katrina</t>
-  </si>
-  <si>
-    <t>Lili works during the daytime while Alberto takes care of Wilfredo, and her favorite part of the day is when they are all at home for an hour. She loves tigers.</t>
-  </si>
-  <si>
-    <t>fixed wheel bicycle</t>
-  </si>
-  <si>
-    <t>ray-ban shades</t>
-  </si>
-  <si>
-    <t>jeans</t>
-  </si>
-  <si>
-    <t>hoodie</t>
-  </si>
-  <si>
-    <t>Wilfredo</t>
-  </si>
-  <si>
-    <t>Will is a happy kid who loves running, jumping, and playing! He also loves octopuses and reading comics.</t>
-  </si>
-  <si>
-    <t>football</t>
-  </si>
-  <si>
-    <t>baseball glove</t>
-  </si>
-  <si>
-    <t>basketball</t>
-  </si>
-  <si>
-    <t>Katy</t>
-  </si>
-  <si>
-    <t>Jesus is a great dad, and loves playing hide and seek with Samuel. He also likes woodworking and video games.</t>
-  </si>
-  <si>
-    <t>Xochitl</t>
-  </si>
-  <si>
-    <t>Frances is a cute toddler with a big smile. She likes dolls and the color red.</t>
-  </si>
-  <si>
-    <t>teddy bear</t>
-  </si>
-  <si>
-    <t>hats</t>
-  </si>
-  <si>
-    <t>Joseph</t>
-  </si>
-  <si>
-    <t>Alejandro is an active little boy, who loves drawing and telling his parents stories. His current favorite color is brown.</t>
-  </si>
-  <si>
-    <t>infant</t>
-  </si>
-  <si>
-    <t>Joseph is a happy baby and loves to smile.</t>
-  </si>
-  <si>
-    <t>Ed is a great dad who loves computers, and has been keeping his old 2000 laptop working for a long time.</t>
-  </si>
-  <si>
-    <t>DR5D</t>
-  </si>
-  <si>
-    <t>yo-yo</t>
-  </si>
-  <si>
-    <t>backpack</t>
-  </si>
-  <si>
-    <t>coffee mugs</t>
-  </si>
-  <si>
-    <t>bbq</t>
-  </si>
-  <si>
-    <t>Ginny</t>
-  </si>
-  <si>
-    <t>Ginny is a hard-working mom, who is always teaching her kids to be kind people. She loves anything orange!</t>
-  </si>
-  <si>
-    <t>pet monkey</t>
-  </si>
-  <si>
-    <t>watch</t>
-  </si>
-  <si>
-    <t>Kelly</t>
-  </si>
-  <si>
-    <t>Kelly loves trucks, monkeys, and her siblings. When she's not running around outside, she loves to sing.</t>
-  </si>
-  <si>
-    <t>pants</t>
-  </si>
-  <si>
-    <t>shirt</t>
-  </si>
-  <si>
-    <t>stuffed animals</t>
-  </si>
-  <si>
-    <t>Isabella</t>
-  </si>
-  <si>
-    <t>Isabella is a smart cookie who loves finger painting, dogs, and Teletubbies.</t>
-  </si>
-  <si>
-    <t>Renata</t>
-  </si>
-  <si>
-    <t>Renatta is working hard to provide for her toddler, Maria, without much family support. When she's not at work she quilts and listens to Taylor Swift.</t>
-  </si>
-  <si>
-    <t>DR5E</t>
-  </si>
-  <si>
-    <t>iron</t>
-  </si>
-  <si>
-    <t>dining table</t>
-  </si>
-  <si>
-    <t>waffle iron</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Maria is a strong little girl who loves ponies, the color red, and playing the ukelele.</t>
-  </si>
-  <si>
-    <t>DR5F</t>
-  </si>
-  <si>
-    <t>Florence</t>
-  </si>
-  <si>
-    <t>Florence works at the hospital, and has been taking college classes to become a nurse. She loves running and playing with her baby.</t>
-  </si>
-  <si>
-    <t>dresses</t>
-  </si>
-  <si>
-    <t>socks</t>
-  </si>
-  <si>
-    <t>bed sheets</t>
-  </si>
-  <si>
-    <t>robe</t>
-  </si>
-  <si>
-    <t>Katy is supporting her kids while working full-time at a local mall. She loves pop cultural analysis and reading feminist blogs.</t>
-  </si>
-  <si>
-    <t>DR5C</t>
-  </si>
-  <si>
-    <t>Chelsea</t>
-  </si>
-  <si>
-    <t>Chelsea's an active little girl who loves playing baseball and running around.</t>
-  </si>
-  <si>
-    <t>hamster</t>
-  </si>
-  <si>
-    <t>kitten</t>
-  </si>
-  <si>
-    <t>puppy</t>
-  </si>
-  <si>
-    <t>fish tank</t>
-  </si>
-  <si>
-    <t>sweater</t>
-  </si>
-  <si>
-    <t>Frances</t>
-  </si>
-  <si>
-    <t>drop_location_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DR5K</t>
-  </si>
-  <si>
-    <t>Virginia recently started taking care of her sister's son, Kenny, in addition to her four little ones. She lives alone but has cousins in the area that can help. She loves non-fiction books and gum.</t>
-  </si>
-  <si>
-    <t>DR5G</t>
-  </si>
-  <si>
-    <t>Kenny</t>
-  </si>
-  <si>
-    <t>code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>blankets</t>
-  </si>
-  <si>
-    <t>educational videos</t>
-  </si>
-  <si>
-    <t>Ed</t>
-  </si>
-  <si>
-    <t>Oakland</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Richmond</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shades</t>
-  </si>
-  <si>
-    <t>swim trunks</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>size_pants</t>
-  </si>
-  <si>
-    <t>size_shirt</t>
-  </si>
-  <si>
-    <t>size_dress</t>
-  </si>
-  <si>
-    <t>size_shoes</t>
-  </si>
-  <si>
-    <t>Antioch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bio</t>
-  </si>
-  <si>
-    <t>need1</t>
-  </si>
-  <si>
-    <t>need2</t>
-  </si>
-  <si>
-    <t>need3</t>
-  </si>
-  <si>
-    <t>need4</t>
-  </si>
-  <si>
-    <t>need5</t>
-  </si>
-  <si>
-    <t>need6</t>
-  </si>
-  <si>
-    <t>Fran</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>Lovely stay-at-home mom attending community college classes and trying to earn her associate's degree. She loves romance novels.</t>
-  </si>
-  <si>
-    <t>DR5A</t>
-  </si>
-  <si>
-    <t>vacuum cleaner</t>
-  </si>
-  <si>
-    <t>dishes</t>
-  </si>
-  <si>
-    <t>pots/pans</t>
-  </si>
-  <si>
-    <t>dress</t>
-  </si>
-  <si>
-    <t>hat</t>
-  </si>
-  <si>
-    <t>couch</t>
-  </si>
-  <si>
-    <t>Phil Jr.</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>small</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>Phil Jr is a lovely, hard-working kid who loves to run around outside and play with his younger sisters.</t>
-  </si>
-  <si>
-    <t>toys</t>
-  </si>
-  <si>
-    <t>art supplies</t>
-  </si>
-  <si>
-    <t>guitar</t>
-  </si>
-  <si>
-    <t>drums</t>
-  </si>
-  <si>
-    <t>Arianna</t>
-  </si>
-  <si>
-    <t>Arianna is a spunky little 6 year old who is obsessed with animals and is learning to read very quickly!</t>
-  </si>
-  <si>
-    <t>legos</t>
-  </si>
-  <si>
-    <t>books</t>
-  </si>
-  <si>
-    <t>shirts</t>
-  </si>
-  <si>
-    <t>shoes</t>
-  </si>
-  <si>
-    <t>Alberto</t>
-  </si>
-  <si>
-    <t>large</t>
-  </si>
-  <si>
-    <t>Alberto loves soap operas and taking care of Wilfredo. He works the night shift at a factory, and takes care of his little girl in the day time.</t>
-  </si>
-  <si>
-    <t>DR5B</t>
-  </si>
-  <si>
-    <t>microwave</t>
-  </si>
-  <si>
-    <t>cd player</t>
-  </si>
-  <si>
-    <t>laptop</t>
-  </si>
-  <si>
-    <t>Lili</t>
   </si>
 </sst>
 </file>
@@ -944,7 +941,7 @@
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
@@ -954,69 +951,69 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>128</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>132</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>133</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>135</v>
+        <v>49</v>
       </c>
       <c r="I1" t="s">
-        <v>119</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
-        <v>114</v>
+        <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="L1" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="M1" t="s">
-        <v>138</v>
+        <v>52</v>
       </c>
       <c r="N1" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="O1" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
       <c r="P1" t="s">
-        <v>141</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
-        <v>142</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="F2" s="1">
         <v>10</v>
@@ -1025,31 +1022,31 @@
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>147</v>
+        <v>60</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>148</v>
+        <v>61</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>149</v>
+        <v>62</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>152</v>
+        <v>65</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -1058,46 +1055,46 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>153</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1">
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1">
         <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G3" s="1">
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>157</v>
+        <v>70</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>158</v>
+        <v>71</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>159</v>
+        <v>72</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1108,13 +1105,13 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
-        <v>162</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1129,28 +1126,28 @@
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>163</v>
+        <v>76</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>165</v>
+        <v>78</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -1160,43 +1157,43 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1">
         <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D5" s="1">
         <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>169</v>
+        <v>82</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G5" s="1">
         <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>172</v>
+        <v>2</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>173</v>
+        <v>3</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>174</v>
+        <v>4</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1208,19 +1205,19 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="1" t="s">
-        <v>175</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D6" s="1">
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="F6" s="1">
         <v>8</v>
@@ -1229,25 +1226,25 @@
         <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1258,13 +1255,13 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
@@ -1273,31 +1270,31 @@
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G7" s="1">
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>171</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>158</v>
+        <v>71</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -1308,19 +1305,19 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="B8">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -1329,36 +1326,36 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>7</v>
+        <v>136</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K8" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="L8" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="M8" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="N8" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1373,39 +1370,39 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>105</v>
+        <v>19</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K9" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="L9" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="M9" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="N9" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="O9" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -1417,140 +1414,140 @@
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="I10" t="s">
-        <v>105</v>
+        <v>19</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K10" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="L10" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="M10" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="N10" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="O10" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="F11" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="H11" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="I11" t="s">
-        <v>105</v>
+        <v>19</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K11" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="L11" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M11" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="N11" t="s">
-        <v>121</v>
+        <v>35</v>
       </c>
       <c r="O11" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1" t="s">
-        <v>122</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1">
         <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D12" s="1">
         <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>169</v>
+        <v>82</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G12" s="1">
         <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>174</v>
+        <v>4</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="B13" s="1">
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="F13" s="1">
         <v>8</v>
@@ -1559,40 +1556,40 @@
         <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="L13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="O13" s="1" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="1" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="B14" s="1">
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
@@ -1607,38 +1604,38 @@
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="1" t="s">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1">
         <v>2</v>
@@ -1653,46 +1650,46 @@
         <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>165</v>
+        <v>78</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="1" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="B16" s="1">
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D16" s="1">
         <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="F16" s="1">
         <v>8</v>
@@ -1701,31 +1698,31 @@
         <v>6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>26</v>
+        <v>154</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>149</v>
+        <v>62</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -1734,13 +1731,13 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="1" t="s">
-        <v>95</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1755,28 +1752,28 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -1786,66 +1783,66 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D18">
         <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>169</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G18">
         <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="I18" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="K18" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="L18" t="s">
-        <v>174</v>
+        <v>4</v>
       </c>
       <c r="M18" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="N18" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="O18" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D19">
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>169</v>
+        <v>82</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -1854,145 +1851,145 @@
         <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="I19" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="K19" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="L19" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="M19" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="N19" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="O19" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="P19" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>137</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="F20" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
       <c r="I20" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="K20" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="L20" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M20" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="N20" t="s">
-        <v>121</v>
+        <v>35</v>
       </c>
       <c r="O20" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="B21">
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D21">
         <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G21">
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>12</v>
+        <v>140</v>
       </c>
       <c r="I21" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="K21" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="L21" t="s">
-        <v>159</v>
+        <v>72</v>
       </c>
       <c r="M21" t="s">
-        <v>14</v>
+        <v>142</v>
       </c>
       <c r="N21" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="O21" t="s">
-        <v>15</v>
+        <v>143</v>
       </c>
       <c r="P21" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>144</v>
       </c>
       <c r="B22" s="1">
         <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1">
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="F22" s="1">
         <v>10</v>
@@ -2001,25 +1998,25 @@
         <v>7</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>116</v>
+        <v>30</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>117</v>
+        <v>31</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>159</v>
+        <v>72</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>14</v>
+        <v>142</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -2030,13 +2027,13 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="1" t="s">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1">
         <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D23" s="1">
         <v>5</v>
@@ -2045,31 +2042,31 @@
         <v>5</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G23" s="1">
         <v>1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>117</v>
+        <v>31</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -2080,13 +2077,13 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>150</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
@@ -2095,37 +2092,37 @@
         <v>4</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>23</v>
+        <v>151</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>117</v>
+        <v>31</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>112</v>
+        <v>26</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>125</v>
+        <v>39</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -2134,13 +2131,13 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="1" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -2155,28 +2152,28 @@
         <v>1</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>27</v>
+        <v>155</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>117</v>
+        <v>31</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -2186,49 +2183,49 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>156</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>29</v>
+        <v>157</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>117</v>
+        <v>31</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>124</v>
+        <v>38</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>121</v>
+        <v>35</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
@@ -2238,49 +2235,49 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>158</v>
       </c>
       <c r="B27" s="1">
         <v>28</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D27" s="1">
         <v>45</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>31</v>
+        <v>159</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G27" s="1">
         <v>10</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>32</v>
+        <v>160</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>33</v>
+        <v>161</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>174</v>
+        <v>4</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>34</v>
+        <v>162</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>35</v>
+        <v>163</v>
       </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -2290,19 +2287,19 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>164</v>
       </c>
       <c r="B28" s="1">
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D28" s="1">
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="F28" s="1">
         <v>10</v>
@@ -2311,31 +2308,31 @@
         <v>4</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>37</v>
+        <v>165</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>33</v>
+        <v>161</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>38</v>
+        <v>166</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -2344,13 +2341,13 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>169</v>
       </c>
       <c r="B29" s="1">
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D29" s="1">
         <v>5</v>
@@ -2359,34 +2356,34 @@
         <v>5</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G29" s="1">
         <v>5</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>33</v>
+        <v>161</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>158</v>
+        <v>71</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>159</v>
+        <v>72</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
@@ -2396,158 +2393,158 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>171</v>
       </c>
       <c r="B30">
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D30">
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="F30" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G30">
         <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>44</v>
+        <v>172</v>
       </c>
       <c r="I30" t="s">
-        <v>45</v>
+        <v>173</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K30" t="s">
-        <v>159</v>
+        <v>72</v>
       </c>
       <c r="L30" t="s">
-        <v>14</v>
+        <v>142</v>
       </c>
       <c r="M30" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="N30" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:20">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>174</v>
       </c>
       <c r="B31">
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D31">
         <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="F31" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G31">
         <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="I31" t="s">
-        <v>45</v>
+        <v>173</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K31" t="s">
-        <v>174</v>
+        <v>4</v>
       </c>
       <c r="L31" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="M31" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="N31" t="s">
-        <v>34</v>
+        <v>162</v>
       </c>
       <c r="O31" t="s">
-        <v>35</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:20">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B32" s="1">
         <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D32" s="1">
         <v>36</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>169</v>
+        <v>82</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G32" s="1">
         <v>12</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>174</v>
+        <v>4</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="P32" s="1"/>
     </row>
     <row r="33" spans="1:20">
       <c r="A33" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B33" s="1">
         <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D33" s="1">
         <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="F33" s="1">
         <v>8</v>
@@ -2556,40 +2553,40 @@
         <v>6</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="L33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="M33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="O33" s="1" t="s">
-        <v>120</v>
+        <v>34</v>
       </c>
       <c r="P33" s="1"/>
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="1" t="s">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="B34" s="1">
         <v>10</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D34" s="1">
         <v>2</v>
@@ -2604,38 +2601,38 @@
         <v>5</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
     <row r="35" spans="1:20">
       <c r="A35" s="1" t="s">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="B35" s="1">
         <v>2</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D35" s="1">
         <v>2</v>
@@ -2650,76 +2647,76 @@
         <v>2</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>150</v>
+        <v>63</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>165</v>
+        <v>78</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>167</v>
+        <v>80</v>
       </c>
       <c r="P35" s="1"/>
     </row>
     <row r="36" spans="1:20">
       <c r="A36" s="1" t="s">
-        <v>3</v>
+        <v>133</v>
       </c>
       <c r="B36" s="1">
         <v>28</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D36" s="1">
         <v>45</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>31</v>
+        <v>159</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G36" s="1">
         <v>10</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>174</v>
+        <v>4</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>34</v>
+        <v>162</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>35</v>
+        <v>163</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -2729,19 +2726,19 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="1" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B37" s="1">
         <v>25</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="D37" s="1">
         <v>10</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="F37" s="1">
         <v>10</v>
@@ -2750,31 +2747,31 @@
         <v>4</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>115</v>
+        <v>29</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>38</v>
+        <v>166</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -2783,13 +2780,13 @@
     </row>
     <row r="38" spans="1:20">
       <c r="A38" s="1" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="B38" s="1">
         <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D38" s="1">
         <v>5</v>
@@ -2798,34 +2795,34 @@
         <v>5</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="G38" s="1">
         <v>5</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>4</v>
+        <v>134</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>158</v>
+        <v>71</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>159</v>
+        <v>72</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
@@ -3274,7 +3271,6 @@
       <c r="T58" s="1"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
change families index to show 4 cards, with only name and age of members
</commit_message>
<xml_diff>
--- a/import_files/full_bios.xlsx
+++ b/import_files/full_bios.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="130000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,14 +19,365 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="181">
+  <si>
+    <t>James recently immigrated to the US to be closer to his partner, Tyler. He's having trouble getting a work visa. He loves puppies and cartoons.</t>
+  </si>
+  <si>
+    <t>Tyler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DR5L    </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5M</t>
+  </si>
+  <si>
+    <t>DR5M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5N</t>
+  </si>
+  <si>
+    <t>DR5N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5O</t>
+  </si>
+  <si>
+    <t>DR5O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5P</t>
+  </si>
+  <si>
+    <t>DR5P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5Q</t>
+  </si>
+  <si>
+    <t>DR5Q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5R</t>
+  </si>
+  <si>
+    <t>DR5R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5S</t>
+  </si>
+  <si>
+    <t>DR5S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5T</t>
+  </si>
+  <si>
+    <t>DR5T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5U</t>
+  </si>
+  <si>
+    <t>DR5U</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR5V</t>
+  </si>
+  <si>
+    <t>DR5V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Renatta is working hard to provide for her toddler, Maria, without much family support. When she's not at work she quilts and listens to Taylor Swift.</t>
+  </si>
+  <si>
+    <t>iron</t>
+  </si>
+  <si>
+    <t>dining table</t>
+  </si>
+  <si>
+    <t>Katrina is a hard-working mom, who is always teaching her kids to be kind people. She loves anything orange!</t>
+  </si>
+  <si>
+    <t>Sabrina</t>
+  </si>
+  <si>
+    <t>Sabrina loves trucks, monkeys, and her siblings. When she's not running around outside, she loves to sing.</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>Lloyd</t>
+  </si>
+  <si>
+    <t>Lloyd is a little baby with a big personality. Ed loves to dress him up in flowery onesies.</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>TJ loves baseball, basketball, and animals. His favorite color is orange.</t>
+  </si>
+  <si>
+    <t>rap CDs</t>
+  </si>
+  <si>
+    <t>t shirts</t>
+  </si>
+  <si>
+    <t>belts</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oakland  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oakland</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xochi is working on getting her associate's degree part time, and spends every free moment she can with Samuel and Mateo. She loves to cook and listen to opera.</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Kenny is just learning to read, and loves it. He also loves kittens and the color blue.</t>
+  </si>
+  <si>
+    <t>Freddy</t>
+  </si>
+  <si>
+    <t>Freddy looks up to his big brother Kenny, and loves playing in the dirt.</t>
+  </si>
+  <si>
+    <t>onesie</t>
+  </si>
+  <si>
+    <t>Antioch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oakland</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kelly is a rambuncious toddler who loves peas, clocks, and hats.</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Jane is a happy little baby, who loves tickles, snuggles, and sleep.</t>
+  </si>
+  <si>
+    <t>Mateo</t>
+  </si>
+  <si>
+    <t>xxl</t>
+  </si>
+  <si>
+    <t>Mateo is a great dad, and loves playing hide and seek with Samuel. He also likes woodworking and video games.</t>
+  </si>
+  <si>
+    <t>blanket</t>
+  </si>
+  <si>
+    <t>bluray player</t>
+  </si>
+  <si>
+    <t>Jasmin</t>
+  </si>
+  <si>
+    <t>Jasmin is working on getting her associate's degree part time, and spends every free moment she can with Samuel and Mateo. She loves to cook and listen to opera.</t>
+  </si>
+  <si>
+    <t>mini fridge</t>
+  </si>
+  <si>
+    <t>cookware</t>
+  </si>
+  <si>
+    <t>alarm clock</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>Samuel is an active little boy, who loves drawing and telling his parents stories. His current favorite color is brown.</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Arianna</t>
+  </si>
+  <si>
+    <t>Arianna is a spunky little 6 year old who is obsessed with animals and is learning to read very quickly!</t>
+  </si>
+  <si>
+    <t>legos</t>
+  </si>
+  <si>
+    <t>books</t>
+  </si>
+  <si>
+    <t>shirts</t>
+  </si>
+  <si>
+    <t>shoes</t>
+  </si>
+  <si>
+    <t>Alberto</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>Tyler works part-time due to a physical limitation, and isn't able to earn a full salary. He's currently supporting Tyler and himself, and loves the color green and the outdoors.</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Fred is a great dad who loves computers, and has been keeping his old 2000 laptop working for a long time.</t>
+  </si>
+  <si>
+    <t>Katrina</t>
+  </si>
+  <si>
+    <t>Lili works during the daytime while Alberto takes care of Wilfredo, and her favorite part of the day is when they are all at home for an hour. She loves tigers.</t>
+  </si>
+  <si>
+    <t>fixed wheel bicycle</t>
+  </si>
+  <si>
+    <t>ray-ban shades</t>
+  </si>
+  <si>
+    <t>jeans</t>
+  </si>
+  <si>
+    <t>hoodie</t>
+  </si>
+  <si>
+    <t>Wilfredo</t>
+  </si>
+  <si>
+    <t>Will is a happy kid who loves running, jumping, and playing! He also loves octopuses and reading comics.</t>
+  </si>
+  <si>
+    <t>football</t>
+  </si>
+  <si>
+    <t>baseball glove</t>
+  </si>
+  <si>
+    <t>basketball</t>
+  </si>
+  <si>
+    <t>Katy</t>
+  </si>
+  <si>
+    <t>Jesus is a great dad, and loves playing hide and seek with Samuel. He also likes woodworking and video games.</t>
+  </si>
+  <si>
+    <t>Xochitl</t>
+  </si>
+  <si>
+    <t>Frances is a cute toddler with a big smile. She likes dolls and the color red.</t>
+  </si>
+  <si>
+    <t>teddy bear</t>
+  </si>
+  <si>
+    <t>hats</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Alejandro is an active little boy, who loves drawing and telling his parents stories. His current favorite color is brown.</t>
+  </si>
+  <si>
+    <t>infant</t>
+  </si>
+  <si>
+    <t>Joseph is a happy baby and loves to smile.</t>
+  </si>
+  <si>
+    <t>Ed is a great dad who loves computers, and has been keeping his old 2000 laptop working for a long time.</t>
+  </si>
+  <si>
+    <t>yo-yo</t>
+  </si>
+  <si>
+    <t>backpack</t>
+  </si>
+  <si>
+    <t>coffee mugs</t>
+  </si>
+  <si>
+    <t>bbq</t>
+  </si>
+  <si>
+    <t>Ginny</t>
+  </si>
+  <si>
+    <t>Ginny is a hard-working mom, who is always teaching her kids to be kind people. She loves anything orange!</t>
+  </si>
+  <si>
+    <t>pet monkey</t>
+  </si>
+  <si>
+    <t>watch</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Kelly loves trucks, monkeys, and her siblings. When she's not running around outside, she loves to sing.</t>
+  </si>
+  <si>
+    <t>pants</t>
+  </si>
+  <si>
+    <t>shirt</t>
+  </si>
+  <si>
+    <t>stuffed animals</t>
+  </si>
+  <si>
+    <t>Isabella</t>
+  </si>
+  <si>
+    <t>Isabella is a smart cookie who loves finger painting, dogs, and Teletubbies.</t>
+  </si>
+  <si>
+    <t>Renata</t>
+  </si>
   <si>
     <t>Alberto loves soap operas and taking care of Wilfredo. He works the night shift at a factory, and takes care of his little girl in the day time.</t>
   </si>
   <si>
-    <t>DR5B</t>
-  </si>
-  <si>
     <t>microwave</t>
   </si>
   <si>
@@ -39,14 +390,6 @@
     <t>Lili</t>
   </si>
   <si>
-    <t xml:space="preserve">DR5A    </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DR5A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>waffle iron</t>
   </si>
   <si>
@@ -56,9 +399,6 @@
     <t>Maria is a strong little girl who loves ponies, the color red, and playing the ukelele.</t>
   </si>
   <si>
-    <t>DR5F</t>
-  </si>
-  <si>
     <t>Florence</t>
   </si>
   <si>
@@ -78,9 +418,6 @@
   </si>
   <si>
     <t>Katy is supporting her kids while working full-time at a local mall. She loves pop cultural analysis and reading feminist blogs.</t>
-  </si>
-  <si>
-    <t>DR5C</t>
   </si>
   <si>
     <t>Chelsea</t>
@@ -111,13 +448,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DR5K</t>
-  </si>
-  <si>
     <t>Virginia recently started taking care of her sister's son, Kenny, in addition to her four little ones. She lives alone but has cousins in the area that can help. She loves non-fiction books and gum.</t>
-  </si>
-  <si>
-    <t>DR5G</t>
   </si>
   <si>
     <t>Kenny</t>
@@ -251,313 +582,6 @@
   </si>
   <si>
     <t>drums</t>
-  </si>
-  <si>
-    <t>Arianna</t>
-  </si>
-  <si>
-    <t>Arianna is a spunky little 6 year old who is obsessed with animals and is learning to read very quickly!</t>
-  </si>
-  <si>
-    <t>legos</t>
-  </si>
-  <si>
-    <t>books</t>
-  </si>
-  <si>
-    <t>shirts</t>
-  </si>
-  <si>
-    <t>shoes</t>
-  </si>
-  <si>
-    <t>Alberto</t>
-  </si>
-  <si>
-    <t>large</t>
-  </si>
-  <si>
-    <t>Tyler works part-time due to a physical limitation, and isn't able to earn a full salary. He's currently supporting Tyler and himself, and loves the color green and the outdoors.</t>
-  </si>
-  <si>
-    <t>Fred</t>
-  </si>
-  <si>
-    <t>Fred is a great dad who loves computers, and has been keeping his old 2000 laptop working for a long time.</t>
-  </si>
-  <si>
-    <t>DR5J</t>
-  </si>
-  <si>
-    <t>Katrina</t>
-  </si>
-  <si>
-    <t>Lili works during the daytime while Alberto takes care of Wilfredo, and her favorite part of the day is when they are all at home for an hour. She loves tigers.</t>
-  </si>
-  <si>
-    <t>fixed wheel bicycle</t>
-  </si>
-  <si>
-    <t>ray-ban shades</t>
-  </si>
-  <si>
-    <t>jeans</t>
-  </si>
-  <si>
-    <t>hoodie</t>
-  </si>
-  <si>
-    <t>Wilfredo</t>
-  </si>
-  <si>
-    <t>Will is a happy kid who loves running, jumping, and playing! He also loves octopuses and reading comics.</t>
-  </si>
-  <si>
-    <t>football</t>
-  </si>
-  <si>
-    <t>baseball glove</t>
-  </si>
-  <si>
-    <t>basketball</t>
-  </si>
-  <si>
-    <t>Katy</t>
-  </si>
-  <si>
-    <t>Jesus is a great dad, and loves playing hide and seek with Samuel. He also likes woodworking and video games.</t>
-  </si>
-  <si>
-    <t>Xochitl</t>
-  </si>
-  <si>
-    <t>Frances is a cute toddler with a big smile. She likes dolls and the color red.</t>
-  </si>
-  <si>
-    <t>teddy bear</t>
-  </si>
-  <si>
-    <t>hats</t>
-  </si>
-  <si>
-    <t>Joseph</t>
-  </si>
-  <si>
-    <t>Alejandro is an active little boy, who loves drawing and telling his parents stories. His current favorite color is brown.</t>
-  </si>
-  <si>
-    <t>infant</t>
-  </si>
-  <si>
-    <t>Joseph is a happy baby and loves to smile.</t>
-  </si>
-  <si>
-    <t>Ed is a great dad who loves computers, and has been keeping his old 2000 laptop working for a long time.</t>
-  </si>
-  <si>
-    <t>DR5D</t>
-  </si>
-  <si>
-    <t>yo-yo</t>
-  </si>
-  <si>
-    <t>backpack</t>
-  </si>
-  <si>
-    <t>coffee mugs</t>
-  </si>
-  <si>
-    <t>bbq</t>
-  </si>
-  <si>
-    <t>Ginny</t>
-  </si>
-  <si>
-    <t>Ginny is a hard-working mom, who is always teaching her kids to be kind people. She loves anything orange!</t>
-  </si>
-  <si>
-    <t>pet monkey</t>
-  </si>
-  <si>
-    <t>watch</t>
-  </si>
-  <si>
-    <t>Kelly</t>
-  </si>
-  <si>
-    <t>Kelly loves trucks, monkeys, and her siblings. When she's not running around outside, she loves to sing.</t>
-  </si>
-  <si>
-    <t>pants</t>
-  </si>
-  <si>
-    <t>shirt</t>
-  </si>
-  <si>
-    <t>stuffed animals</t>
-  </si>
-  <si>
-    <t>Isabella</t>
-  </si>
-  <si>
-    <t>Isabella is a smart cookie who loves finger painting, dogs, and Teletubbies.</t>
-  </si>
-  <si>
-    <t>Renata</t>
-  </si>
-  <si>
-    <t>Renatta is working hard to provide for her toddler, Maria, without much family support. When she's not at work she quilts and listens to Taylor Swift.</t>
-  </si>
-  <si>
-    <t>DR5E</t>
-  </si>
-  <si>
-    <t>iron</t>
-  </si>
-  <si>
-    <t>dining table</t>
-  </si>
-  <si>
-    <t>Katrina is a hard-working mom, who is always teaching her kids to be kind people. She loves anything orange!</t>
-  </si>
-  <si>
-    <t>Sabrina</t>
-  </si>
-  <si>
-    <t>Sabrina loves trucks, monkeys, and her siblings. When she's not running around outside, she loves to sing.</t>
-  </si>
-  <si>
-    <t>Jesus</t>
-  </si>
-  <si>
-    <t>DR5K</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DR5B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DR5C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lloyd</t>
-  </si>
-  <si>
-    <t>Lloyd is a little baby with a big personality. Ed loves to dress him up in flowery onesies.</t>
-  </si>
-  <si>
-    <t>TJ</t>
-  </si>
-  <si>
-    <t>TJ loves baseball, basketball, and animals. His favorite color is orange.</t>
-  </si>
-  <si>
-    <t>rap CDs</t>
-  </si>
-  <si>
-    <t>t shirts</t>
-  </si>
-  <si>
-    <t>belts</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oakland  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Oakland</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Xochi is working on getting her associate's degree part time, and spends every free moment she can with Samuel and Mateo. She loves to cook and listen to opera.</t>
-  </si>
-  <si>
-    <t>Alejandro</t>
-  </si>
-  <si>
-    <t>Kenny is just learning to read, and loves it. He also loves kittens and the color blue.</t>
-  </si>
-  <si>
-    <t>Freddy</t>
-  </si>
-  <si>
-    <t>Freddy looks up to his big brother Kenny, and loves playing in the dirt.</t>
-  </si>
-  <si>
-    <t>onesie</t>
-  </si>
-  <si>
-    <t>Antioch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Oakland</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kelly is a rambuncious toddler who loves peas, clocks, and hats.</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Jane is a happy little baby, who loves tickles, snuggles, and sleep.</t>
-  </si>
-  <si>
-    <t>Mateo</t>
-  </si>
-  <si>
-    <t>xxl</t>
-  </si>
-  <si>
-    <t>Mateo is a great dad, and loves playing hide and seek with Samuel. He also likes woodworking and video games.</t>
-  </si>
-  <si>
-    <t>DR5H</t>
-  </si>
-  <si>
-    <t>blanket</t>
-  </si>
-  <si>
-    <t>bluray player</t>
-  </si>
-  <si>
-    <t>Jasmin</t>
-  </si>
-  <si>
-    <t>Jasmin is working on getting her associate's degree part time, and spends every free moment she can with Samuel and Mateo. She loves to cook and listen to opera.</t>
-  </si>
-  <si>
-    <t>mini fridge</t>
-  </si>
-  <si>
-    <t>cookware</t>
-  </si>
-  <si>
-    <t>alarm clock</t>
-  </si>
-  <si>
-    <t>Samuel</t>
-  </si>
-  <si>
-    <t>Samuel is an active little boy, who loves drawing and telling his parents stories. His current favorite color is brown.</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>James recently immigrated to the US to be closer to his partner, Tyler. He's having trouble getting a work visa. He loves puppies and cartoons.</t>
-  </si>
-  <si>
-    <t>DR5I</t>
-  </si>
-  <si>
-    <t>Tyler</t>
   </si>
 </sst>
 </file>
@@ -941,7 +965,7 @@
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1"/>
@@ -951,69 +975,69 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>150</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>151</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="H1" t="s">
-        <v>49</v>
+        <v>155</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="K1" t="s">
-        <v>50</v>
+        <v>156</v>
       </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="M1" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="N1" t="s">
-        <v>53</v>
+        <v>159</v>
       </c>
       <c r="O1" t="s">
-        <v>54</v>
+        <v>160</v>
       </c>
       <c r="P1" t="s">
-        <v>55</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>162</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="F2" s="1">
         <v>10</v>
@@ -1022,31 +1046,31 @@
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>59</v>
+        <v>165</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>145</v>
+        <v>38</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>61</v>
+        <v>167</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>62</v>
+        <v>168</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>64</v>
+        <v>170</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>65</v>
+        <v>171</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -1055,46 +1079,46 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>172</v>
       </c>
       <c r="B3" s="1">
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D3" s="1">
         <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>68</v>
+        <v>174</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G3" s="1">
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>70</v>
+        <v>176</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>146</v>
+        <v>39</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>71</v>
+        <v>177</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>72</v>
+        <v>178</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>74</v>
+        <v>180</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1105,13 +1129,13 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -1126,28 +1150,28 @@
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -1157,43 +1181,43 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1">
         <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D5" s="1">
         <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G5" s="1">
         <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1205,19 +1229,19 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1">
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D6" s="1">
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>68</v>
+        <v>174</v>
       </c>
       <c r="F6" s="1">
         <v>8</v>
@@ -1226,25 +1250,25 @@
         <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>135</v>
+        <v>3</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1255,13 +1279,13 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
@@ -1270,31 +1294,31 @@
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G7" s="1">
         <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>71</v>
+        <v>177</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -1305,19 +1329,19 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B8">
         <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>174</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -1326,36 +1350,36 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>127</v>
       </c>
       <c r="I8" t="s">
-        <v>136</v>
+        <v>6</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="L8" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="M8" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="N8" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1370,39 +1394,39 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="I9" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K9" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
       <c r="L9" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="M9" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>133</v>
       </c>
       <c r="O9" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -1414,140 +1438,140 @@
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K10" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="L10" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="M10" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="N10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="O10" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="H11" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K11" t="s">
-        <v>152</v>
+        <v>45</v>
       </c>
       <c r="L11" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="N11" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
       <c r="O11" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="B12" s="1">
         <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D12" s="1">
         <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G12" s="1">
         <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B13" s="1">
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D13" s="1">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="F13" s="1">
         <v>8</v>
@@ -1556,40 +1580,40 @@
         <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B14" s="1">
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D14" s="1">
         <v>2</v>
@@ -1604,38 +1628,38 @@
         <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D15" s="1">
         <v>2</v>
@@ -1650,46 +1674,46 @@
         <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="1" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B16" s="1">
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D16" s="1">
         <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>174</v>
       </c>
       <c r="F16" s="1">
         <v>8</v>
@@ -1698,31 +1722,31 @@
         <v>6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>126</v>
+        <v>23</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>154</v>
+        <v>47</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>128</v>
+        <v>24</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>62</v>
+        <v>168</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -1731,13 +1755,13 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1752,28 +1776,28 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -1783,66 +1807,66 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="B18">
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D18">
         <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G18">
         <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="I18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="K18" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="L18" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="M18" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="N18" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="O18" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="B19">
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D19">
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -1851,145 +1875,145 @@
         <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="K19" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="L19" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="M19" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="N19" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="O19" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="P19" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D20" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G20" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="H20" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
       <c r="I20" t="s">
         <v>11</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="K20" t="s">
-        <v>152</v>
+        <v>45</v>
       </c>
       <c r="L20" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M20" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="N20" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
       <c r="O20" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D21">
         <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G21">
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>140</v>
+        <v>33</v>
       </c>
       <c r="I21" t="s">
         <v>11</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="K21" t="s">
-        <v>141</v>
+        <v>34</v>
       </c>
       <c r="L21" t="s">
-        <v>72</v>
+        <v>178</v>
       </c>
       <c r="M21" t="s">
-        <v>142</v>
+        <v>35</v>
       </c>
       <c r="N21" t="s">
+        <v>79</v>
+      </c>
+      <c r="O21" t="s">
+        <v>36</v>
+      </c>
+      <c r="P21" t="s">
         <v>91</v>
-      </c>
-      <c r="O21" t="s">
-        <v>143</v>
-      </c>
-      <c r="P21" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="1" t="s">
-        <v>144</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1">
         <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D22" s="1">
         <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="F22" s="1">
         <v>10</v>
@@ -1998,25 +2022,25 @@
         <v>7</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>72</v>
+        <v>178</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>142</v>
+        <v>35</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -2027,13 +2051,13 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="B23" s="1">
         <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D23" s="1">
         <v>5</v>
@@ -2042,31 +2066,31 @@
         <v>5</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G23" s="1">
         <v>1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>149</v>
+        <v>42</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -2077,13 +2101,13 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="1" t="s">
-        <v>150</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
@@ -2092,37 +2116,37 @@
         <v>4</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>151</v>
+        <v>44</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>39</v>
+        <v>145</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -2131,13 +2155,13 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="1" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -2152,28 +2176,28 @@
         <v>1</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>155</v>
+        <v>48</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -2183,49 +2207,49 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="1" t="s">
-        <v>156</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>157</v>
+        <v>50</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>152</v>
+        <v>45</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>35</v>
+        <v>141</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
@@ -2235,49 +2259,49 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="1" t="s">
-        <v>158</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1">
         <v>28</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D27" s="1">
         <v>45</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>159</v>
+        <v>52</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G27" s="1">
         <v>10</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>161</v>
+        <v>16</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>163</v>
+        <v>55</v>
       </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -2287,19 +2311,19 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="1" t="s">
-        <v>164</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1">
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D28" s="1">
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="F28" s="1">
         <v>10</v>
@@ -2308,31 +2332,31 @@
         <v>4</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>165</v>
+        <v>57</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>166</v>
+        <v>58</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>167</v>
+        <v>59</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>168</v>
+        <v>60</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
@@ -2341,13 +2365,13 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="1" t="s">
-        <v>169</v>
+        <v>61</v>
       </c>
       <c r="B29" s="1">
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D29" s="1">
         <v>5</v>
@@ -2356,34 +2380,34 @@
         <v>5</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G29" s="1">
         <v>5</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>170</v>
+        <v>62</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>71</v>
+        <v>177</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>72</v>
+        <v>178</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>74</v>
+        <v>180</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
@@ -2393,158 +2417,158 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" t="s">
-        <v>171</v>
+        <v>63</v>
       </c>
       <c r="B30">
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D30">
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G30">
         <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>173</v>
+        <v>18</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K30" t="s">
-        <v>72</v>
+        <v>178</v>
       </c>
       <c r="L30" t="s">
-        <v>142</v>
+        <v>35</v>
       </c>
       <c r="M30" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="N30" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:20">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>1</v>
       </c>
       <c r="B31">
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D31">
         <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G31">
         <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="I31" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K31" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="L31" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="M31" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="N31" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="O31" t="s">
-        <v>163</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:20">
       <c r="A32" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B32" s="1">
         <v>35</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D32" s="1">
         <v>36</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G32" s="1">
         <v>12</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="P32" s="1"/>
     </row>
     <row r="33" spans="1:20">
       <c r="A33" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B33" s="1">
         <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D33" s="1">
         <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="F33" s="1">
         <v>8</v>
@@ -2553,40 +2577,40 @@
         <v>6</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>130</v>
+        <v>26</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="P33" s="1"/>
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="1" t="s">
-        <v>131</v>
+        <v>27</v>
       </c>
       <c r="B34" s="1">
         <v>10</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D34" s="1">
         <v>2</v>
@@ -2601,38 +2625,38 @@
         <v>5</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
     <row r="35" spans="1:20">
       <c r="A35" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B35" s="1">
         <v>2</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D35" s="1">
         <v>2</v>
@@ -2647,76 +2671,76 @@
         <v>2</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="P35" s="1"/>
     </row>
     <row r="36" spans="1:20">
       <c r="A36" s="1" t="s">
-        <v>133</v>
+        <v>29</v>
       </c>
       <c r="B36" s="1">
         <v>28</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D36" s="1">
         <v>45</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>159</v>
+        <v>52</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G36" s="1">
         <v>10</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>162</v>
+        <v>54</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>163</v>
+        <v>55</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -2726,19 +2750,19 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B37" s="1">
         <v>25</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
       <c r="D37" s="1">
         <v>10</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
       <c r="F37" s="1">
         <v>10</v>
@@ -2747,31 +2771,31 @@
         <v>4</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>147</v>
+        <v>40</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>166</v>
+        <v>58</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>167</v>
+        <v>59</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>168</v>
+        <v>60</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -2780,13 +2804,13 @@
     </row>
     <row r="38" spans="1:20">
       <c r="A38" s="1" t="s">
-        <v>148</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1">
         <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="D38" s="1">
         <v>5</v>
@@ -2795,34 +2819,34 @@
         <v>5</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
       <c r="G38" s="1">
         <v>5</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>153</v>
+        <v>46</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>71</v>
+        <v>177</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>72</v>
+        <v>178</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>74</v>
+        <v>180</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
@@ -3273,6 +3297,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>